<commit_message>
uploading trial time series ARIMA prediction model
</commit_message>
<xml_diff>
--- a/Initial_Data_Analysis.xlsx
+++ b/Initial_Data_Analysis.xlsx
@@ -418,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -533,6 +531,21 @@
       <c r="I7" s="2">
         <v>3.1432000000000002E-2</v>
       </c>
+      <c r="J7" s="2">
+        <v>0.198185</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-0.31230999999999998</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.239288</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2.7486709999999999</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.23070599999999999</v>
+      </c>
     </row>
     <row r="8" spans="2:14">
       <c r="C8" s="2">
@@ -556,6 +569,21 @@
       <c r="I8" s="2">
         <v>6.0070999999999999E-2</v>
       </c>
+      <c r="J8" s="2">
+        <v>-8.7690429999999999</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-0.38095699999999999</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.27910499999999999</v>
+      </c>
+      <c r="M8" s="2">
+        <v>2.6624430000000001</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.14523</v>
+      </c>
     </row>
     <row r="9" spans="2:14">
       <c r="C9" s="2">
@@ -579,6 +607,21 @@
       <c r="I9" s="2">
         <v>5.7945999999999998E-2</v>
       </c>
+      <c r="J9" s="2">
+        <v>-27.300940000000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>-0.33374599999999999</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.35228700000000002</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2.5902859999999999</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.19728000000000001</v>
+      </c>
     </row>
     <row r="10" spans="2:14">
       <c r="C10" s="2">
@@ -602,6 +645,21 @@
       <c r="I10" s="2">
         <v>0.21917</v>
       </c>
+      <c r="J10" s="2">
+        <v>0.21156800000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>-0.28290799999999999</v>
+      </c>
+      <c r="L10" s="2">
+        <v>-2.7186059999999999</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2.6266829999999999</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.10732700000000001</v>
+      </c>
     </row>
     <row r="11" spans="2:14">
       <c r="C11" s="2">
@@ -625,6 +683,21 @@
       <c r="I11" s="2">
         <v>0.23531099999999999</v>
       </c>
+      <c r="J11" s="2">
+        <v>0.21166299999999999</v>
+      </c>
+      <c r="K11" s="2">
+        <v>-0.25428000000000001</v>
+      </c>
+      <c r="L11" s="2">
+        <v>-2.2063540000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>-0.325374</v>
+      </c>
+      <c r="N11" s="2">
+        <v>8.1478999999999996E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:14">
       <c r="C12" s="2">
@@ -648,6 +721,21 @@
       <c r="I12" s="2">
         <v>0.26867999999999997</v>
       </c>
+      <c r="J12" s="2">
+        <v>0.25683800000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>-0.21962699999999999</v>
+      </c>
+      <c r="L12" s="2">
+        <v>-2.0876570000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2.5465909999999998</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.263241</v>
+      </c>
     </row>
     <row r="13" spans="2:14">
       <c r="C13" s="2">
@@ -671,6 +759,21 @@
       <c r="I13" s="2">
         <v>0.100496</v>
       </c>
+      <c r="J13" s="2">
+        <v>0.299759</v>
+      </c>
+      <c r="K13" s="2">
+        <v>-0.21563399999999999</v>
+      </c>
+      <c r="L13" s="2">
+        <v>-2.0615060000000001</v>
+      </c>
+      <c r="M13" s="2">
+        <v>-0.25722</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.19262099999999999</v>
+      </c>
     </row>
     <row r="14" spans="2:14">
       <c r="C14" s="2">
@@ -694,6 +797,21 @@
       <c r="I14" s="2">
         <v>0.17221500000000001</v>
       </c>
+      <c r="J14" s="2">
+        <v>0.26556800000000003</v>
+      </c>
+      <c r="K14" s="2">
+        <v>-0.149672</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-1.0690980000000001</v>
+      </c>
+      <c r="M14" s="2">
+        <v>-0.21726000000000001</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5.3763999999999999E-2</v>
+      </c>
     </row>
     <row r="15" spans="2:14">
       <c r="C15" s="2">
@@ -717,6 +835,21 @@
       <c r="I15" s="2">
         <v>0.132386</v>
       </c>
+      <c r="J15" s="2">
+        <v>0.26360600000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>-0.113693</v>
+      </c>
+      <c r="L15" s="2">
+        <v>9.0723999999999999E-2</v>
+      </c>
+      <c r="M15" s="2">
+        <v>-0.29081099999999999</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.233594</v>
+      </c>
     </row>
     <row r="16" spans="2:14">
       <c r="C16" s="2">
@@ -740,8 +873,23 @@
       <c r="I16" s="2">
         <v>0.173509</v>
       </c>
-    </row>
-    <row r="17" spans="3:9">
+      <c r="J16" s="2">
+        <v>0.27229500000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>-0.249056</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.24241599999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>-0.31922600000000001</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.39887099999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14">
       <c r="C17" s="2">
         <v>5.0024629999999997</v>
       </c>
@@ -763,8 +911,23 @@
       <c r="I17" s="2">
         <v>0.17641999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="3:9">
+      <c r="J17" s="2">
+        <v>0.33257399999999998</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-0.22825000000000001</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.49095899999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <v>-0.48431099999999999</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.373417</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14">
       <c r="C18" s="2">
         <v>3.2428379999999999</v>
       </c>
@@ -786,8 +949,23 @@
       <c r="I18" s="2">
         <v>-1.01E-3</v>
       </c>
-    </row>
-    <row r="19" spans="3:9">
+      <c r="J18" s="2">
+        <v>0.44894299999999998</v>
+      </c>
+      <c r="K18" s="2">
+        <v>-0.19995199999999999</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.47162799999999999</v>
+      </c>
+      <c r="M18" s="2">
+        <v>-0.58790799999999999</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.30244399999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
       <c r="C19" s="2">
         <v>0.28927599999999998</v>
       </c>
@@ -809,8 +987,23 @@
       <c r="I19" s="2">
         <v>0.248333</v>
       </c>
-    </row>
-    <row r="20" spans="3:9">
+      <c r="J19" s="2">
+        <v>0.35874499999999998</v>
+      </c>
+      <c r="K19" s="2">
+        <v>-0.10141</v>
+      </c>
+      <c r="L19" s="2">
+        <v>-0.48861300000000002</v>
+      </c>
+      <c r="M19" s="2">
+        <v>-0.79527400000000004</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.41719800000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
       <c r="C20" s="2">
         <v>0.25277300000000003</v>
       </c>
@@ -832,8 +1025,23 @@
       <c r="I20" s="2">
         <v>0.15546399999999999</v>
       </c>
-    </row>
-    <row r="21" spans="3:9">
+      <c r="J20" s="2">
+        <v>0.31965300000000002</v>
+      </c>
+      <c r="K20" s="2">
+        <v>-0.153805</v>
+      </c>
+      <c r="L20" s="2">
+        <v>-1.844509</v>
+      </c>
+      <c r="M20" s="2">
+        <v>-0.760351</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0.68149000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14">
       <c r="C21" s="2">
         <v>0.21038699999999999</v>
       </c>
@@ -855,8 +1063,23 @@
       <c r="I21" s="2">
         <v>0.21260299999999999</v>
       </c>
-    </row>
-    <row r="22" spans="3:9">
+      <c r="J21" s="2">
+        <v>0.18399199999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>-0.11443</v>
+      </c>
+      <c r="L21" s="2">
+        <v>-2.2208109999999999</v>
+      </c>
+      <c r="M21" s="2">
+        <v>-0.85921999999999998</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0.57286599999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
       <c r="C22" s="2">
         <v>5.2755580000000002</v>
       </c>
@@ -872,14 +1095,29 @@
       <c r="G22" s="2">
         <v>2.8014070000000002</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>4.846781</v>
       </c>
       <c r="I22" s="2">
         <v>0.29019400000000001</v>
       </c>
-    </row>
-    <row r="23" spans="3:9">
+      <c r="J22" s="2">
+        <v>0.23410600000000001</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.18471399999999999</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.5299320000000001</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1.629775</v>
+      </c>
+      <c r="N22" s="2">
+        <v>2.0498980000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
       <c r="C23" s="3">
         <v>8.5485489999999995</v>
       </c>
@@ -889,20 +1127,35 @@
       <c r="E23" s="2">
         <v>3.287712</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="3">
         <v>5.5525349999999998</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>8.1567539999999994</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <v>18.454561999999999</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
         <v>1.6767650000000001</v>
       </c>
-    </row>
-    <row r="24" spans="3:9">
+      <c r="J23" s="2">
+        <v>-0.192249</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3.3923540000000001</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4.7075490000000002</v>
+      </c>
+      <c r="M23" s="2">
+        <v>2.5702349999999998</v>
+      </c>
+      <c r="N23" s="3">
+        <v>6.095529</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
       <c r="C24" s="2">
         <v>-8.6788830000000008</v>
       </c>
@@ -912,20 +1165,35 @@
       <c r="E24" s="2">
         <v>5.1782539999999999</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="3">
         <v>7.941827</v>
       </c>
       <c r="G24" s="2">
         <v>-1.621132</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="3">
         <v>30.077506</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
         <v>1.495242</v>
       </c>
-    </row>
-    <row r="25" spans="3:9">
+      <c r="J24" s="2">
+        <v>-1.1883680000000001</v>
+      </c>
+      <c r="K24" s="3">
+        <v>5.2424299999999997</v>
+      </c>
+      <c r="L24" s="3">
+        <v>5.1648909999999999</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5.5822710000000004</v>
+      </c>
+      <c r="N24" s="3">
+        <v>10.548679999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
       <c r="C25" s="3">
         <v>10.932235</v>
       </c>
@@ -935,20 +1203,35 @@
       <c r="E25" s="2">
         <v>6.5774400000000002</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="3">
         <v>9.9608019999999993</v>
       </c>
       <c r="G25" s="2">
         <v>-2.3189769999999998</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>41.752296999999999</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
         <v>1.4356370000000001</v>
       </c>
-    </row>
-    <row r="26" spans="3:9">
+      <c r="J25" s="2">
+        <v>-1.7638929999999999</v>
+      </c>
+      <c r="K25" s="3">
+        <v>6.7136240000000003</v>
+      </c>
+      <c r="L25" s="3">
+        <v>8.8616510000000002</v>
+      </c>
+      <c r="M25" s="3">
+        <v>7.9875489999999996</v>
+      </c>
+      <c r="N25" s="3">
+        <v>11.304500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
       <c r="C26" s="3">
         <v>13.904157</v>
       </c>
@@ -958,20 +1241,35 @@
       <c r="E26" s="3">
         <v>10.445456999999999</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="3">
         <v>11.5799</v>
       </c>
       <c r="G26" s="2">
         <v>-3.023069</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>53.332830999999999</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
         <v>1.2610710000000001</v>
       </c>
-    </row>
-    <row r="27" spans="3:9">
+      <c r="J26" s="2">
+        <v>-2.3893930000000001</v>
+      </c>
+      <c r="K26" s="3">
+        <v>8.5575039999999998</v>
+      </c>
+      <c r="L26" s="3">
+        <v>8.7297239999999992</v>
+      </c>
+      <c r="M26" s="3">
+        <v>10.072554</v>
+      </c>
+      <c r="N26" s="3">
+        <v>13.433028</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
       <c r="C27" s="2">
         <v>5.3677400000000004</v>
       </c>
@@ -981,20 +1279,35 @@
       <c r="E27" s="3">
         <v>11.524224999999999</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="3">
         <v>12.952455</v>
       </c>
       <c r="G27" s="2">
         <v>-3.7054749999999999</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <v>60.037266000000002</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <v>1.2275149999999999</v>
       </c>
-    </row>
-    <row r="28" spans="3:9">
+      <c r="J27" s="2">
+        <v>-3.2682099999999998</v>
+      </c>
+      <c r="K27" s="3">
+        <v>8.9991090000000007</v>
+      </c>
+      <c r="L27" s="3">
+        <v>13.513112</v>
+      </c>
+      <c r="M27" s="3">
+        <v>11.721772</v>
+      </c>
+      <c r="N27" s="3">
+        <v>15.265772999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
       <c r="C28" s="3">
         <v>19.491105999999998</v>
       </c>
@@ -1004,20 +1317,35 @@
       <c r="E28" s="3">
         <v>12.3727</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="3">
         <v>14.590888</v>
       </c>
       <c r="G28" s="2">
         <v>-4.3083980000000004</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>64.707331999999994</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
         <v>1.1920010000000001</v>
       </c>
-    </row>
-    <row r="29" spans="3:9">
+      <c r="J28" s="2">
+        <v>-3.3102610000000001</v>
+      </c>
+      <c r="K28" s="3">
+        <v>9.6347869999999993</v>
+      </c>
+      <c r="L28" s="3">
+        <v>15.119624</v>
+      </c>
+      <c r="M28" s="3">
+        <v>13.074434999999999</v>
+      </c>
+      <c r="N28" s="3">
+        <v>16.958817</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
       <c r="C29" s="3">
         <v>16.106985000000002</v>
       </c>
@@ -1027,20 +1355,35 @@
       <c r="E29" s="3">
         <v>10.359807999999999</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
         <v>15.466398999999999</v>
       </c>
       <c r="G29" s="2">
         <v>-1.5879909999999999</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <v>67.479484999999997</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <v>1.216494</v>
       </c>
-    </row>
-    <row r="30" spans="3:9">
+      <c r="J29" s="2">
+        <v>-3.5963419999999999</v>
+      </c>
+      <c r="K29" s="3">
+        <v>10.074821</v>
+      </c>
+      <c r="L29" s="3">
+        <v>16.472695999999999</v>
+      </c>
+      <c r="M29" s="3">
+        <v>14.775392999999999</v>
+      </c>
+      <c r="N29" s="3">
+        <v>18.528184</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
       <c r="C30" s="3">
         <v>17.095763000000002</v>
       </c>
@@ -1050,20 +1393,35 @@
       <c r="E30" s="3">
         <v>11.658396</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="3">
         <v>16.273094</v>
       </c>
       <c r="G30" s="2">
         <v>-4.9564529999999998</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <v>72.078417000000002</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
         <v>1.187489</v>
       </c>
-    </row>
-    <row r="31" spans="3:9">
+      <c r="J30" s="2">
+        <v>-3.9315820000000001</v>
+      </c>
+      <c r="K30" s="3">
+        <v>10.591452</v>
+      </c>
+      <c r="L30" s="3">
+        <v>21.465502999999998</v>
+      </c>
+      <c r="M30" s="3">
+        <v>15.501345000000001</v>
+      </c>
+      <c r="N30" s="3">
+        <v>20.592317999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14">
       <c r="C31" s="3">
         <v>17.972626000000002</v>
       </c>
@@ -1073,20 +1431,35 @@
       <c r="E31" s="3">
         <v>11.842670999999999</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="3">
         <v>16.921050000000001</v>
       </c>
       <c r="G31" s="2">
         <v>-5.1485450000000004</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <v>76.057740999999993</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
         <v>1.1259870000000001</v>
       </c>
-    </row>
-    <row r="32" spans="3:9">
+      <c r="J31" s="2">
+        <v>-4.2770010000000003</v>
+      </c>
+      <c r="K31" s="3">
+        <v>11.164596</v>
+      </c>
+      <c r="L31" s="3">
+        <v>20.841277000000002</v>
+      </c>
+      <c r="M31" s="3">
+        <v>16.39536</v>
+      </c>
+      <c r="N31" s="3">
+        <v>20.790599</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14">
       <c r="C32" s="3">
         <v>18.692540999999999</v>
       </c>
@@ -1096,20 +1469,35 @@
       <c r="E32" s="3">
         <v>12.665702</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="3">
         <v>17.546329</v>
       </c>
       <c r="G32" s="2">
         <v>-5.2314559999999997</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <v>79.336943000000005</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="3">
         <v>1.1803809999999999</v>
       </c>
-    </row>
-    <row r="33" spans="3:9">
+      <c r="J32" s="2">
+        <v>-4.4849119999999996</v>
+      </c>
+      <c r="K32" s="3">
+        <v>11.856619</v>
+      </c>
+      <c r="L32" s="3">
+        <v>20.924683999999999</v>
+      </c>
+      <c r="M32" s="3">
+        <v>17.175944999999999</v>
+      </c>
+      <c r="N32" s="3">
+        <v>21.598248999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14">
       <c r="C33" s="3">
         <v>28.397832999999999</v>
       </c>
@@ -1119,20 +1507,35 @@
       <c r="E33" s="3">
         <v>13.390738000000001</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="3">
         <v>18.062866</v>
       </c>
       <c r="G33" s="2">
         <v>-5.3760919999999999</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <v>82.762861000000001</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="3">
         <v>1.234648</v>
       </c>
-    </row>
-    <row r="34" spans="3:9">
+      <c r="J33" s="2">
+        <v>-4.5758530000000004</v>
+      </c>
+      <c r="K33" s="3">
+        <v>12.565979</v>
+      </c>
+      <c r="L33" s="3">
+        <v>19.174683999999999</v>
+      </c>
+      <c r="M33" s="3">
+        <v>17.866091999999998</v>
+      </c>
+      <c r="N33" s="3">
+        <v>22.444849999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14">
       <c r="C34" s="3">
         <v>18.969629000000001</v>
       </c>
@@ -1142,20 +1545,35 @@
       <c r="E34" s="3">
         <v>13.846764</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="3">
         <v>18.285819</v>
       </c>
       <c r="G34" s="2">
         <v>-2.370946</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>80.580483000000001</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="3">
         <v>1.173929</v>
       </c>
-    </row>
-    <row r="35" spans="3:9">
+      <c r="J34" s="2">
+        <v>-4.3077350000000001</v>
+      </c>
+      <c r="K34" s="3">
+        <v>12.823935000000001</v>
+      </c>
+      <c r="L34" s="3">
+        <v>19.708542999999999</v>
+      </c>
+      <c r="M34" s="3">
+        <v>18.478532000000001</v>
+      </c>
+      <c r="N34" s="3">
+        <v>23.038226000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14">
       <c r="C35" s="3">
         <v>17.333960999999999</v>
       </c>
@@ -1165,20 +1583,35 @@
       <c r="E35" s="3">
         <v>13.046673999999999</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="3">
         <v>15.45759</v>
       </c>
       <c r="G35" s="2">
         <v>-2.1016089999999998</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>73.398150999999999</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="3">
         <v>0.98363299999999998</v>
       </c>
-    </row>
-    <row r="36" spans="3:9">
+      <c r="J35" s="2">
+        <v>-4.0876450000000002</v>
+      </c>
+      <c r="K35" s="3">
+        <v>11.511649999999999</v>
+      </c>
+      <c r="L35" s="3">
+        <v>17.368084</v>
+      </c>
+      <c r="M35" s="3">
+        <v>16.443798999999999</v>
+      </c>
+      <c r="N35" s="3">
+        <v>19.591999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14">
       <c r="C36" s="3">
         <v>15.181842</v>
       </c>
@@ -1188,20 +1621,35 @@
       <c r="E36" s="3">
         <v>11.042603</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="3">
         <v>13.184991</v>
       </c>
       <c r="G36" s="2">
         <v>-1.4817199999999999</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <v>63.760803000000003</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="3">
         <v>0.88541999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="3:9">
+      <c r="J36" s="2">
+        <v>-3.4629889999999999</v>
+      </c>
+      <c r="K36" s="3">
+        <v>9.7177399999999992</v>
+      </c>
+      <c r="L36" s="3">
+        <v>16.354558999999998</v>
+      </c>
+      <c r="M36" s="3">
+        <v>14.676849000000001</v>
+      </c>
+      <c r="N36" s="3">
+        <v>17.140729</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14">
       <c r="C37" s="3">
         <v>13.76807</v>
       </c>
@@ -1211,20 +1659,35 @@
       <c r="E37" s="3">
         <v>8.7381960000000003</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="3">
         <v>13.784409999999999</v>
       </c>
       <c r="G37" s="2">
         <v>-3.7494930000000002</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>68.189738000000006</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="3">
         <v>0.937473</v>
       </c>
-    </row>
-    <row r="38" spans="3:9">
+      <c r="J37" s="2">
+        <v>-2.9203830000000002</v>
+      </c>
+      <c r="K37" s="3">
+        <v>8.2804359999999999</v>
+      </c>
+      <c r="L37" s="3">
+        <v>14.093384</v>
+      </c>
+      <c r="M37" s="3">
+        <v>12.474221</v>
+      </c>
+      <c r="N37" s="3">
+        <v>13.728948000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14">
       <c r="C38" s="3">
         <v>12.328626999999999</v>
       </c>
@@ -1240,14 +1703,29 @@
       <c r="G38" s="2">
         <v>-3.1859289999999998</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <v>56.159649000000002</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="3">
         <v>0.861124</v>
       </c>
-    </row>
-    <row r="39" spans="3:9">
+      <c r="J38" s="2">
+        <v>-2.5298720000000001</v>
+      </c>
+      <c r="K38" s="3">
+        <v>7.1252649999999997</v>
+      </c>
+      <c r="L38" s="3">
+        <v>11.014764</v>
+      </c>
+      <c r="M38" s="3">
+        <v>10.357218</v>
+      </c>
+      <c r="N38" s="3">
+        <v>12.714987000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14">
       <c r="C39" s="3">
         <v>9.6792789999999993</v>
       </c>
@@ -1257,20 +1735,35 @@
       <c r="E39" s="2">
         <v>6.8738440000000001</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="3">
         <v>7.7450200000000002</v>
       </c>
       <c r="G39" s="2">
         <v>-2.6660819999999998</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <v>46.525391999999997</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="3">
         <v>0.76209000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="3:9">
+      <c r="J39" s="2">
+        <v>-2.2385769999999998</v>
+      </c>
+      <c r="K39" s="3">
+        <v>5.4290000000000003</v>
+      </c>
+      <c r="L39" s="3">
+        <v>10.240242</v>
+      </c>
+      <c r="M39" s="3">
+        <v>8.6270629999999997</v>
+      </c>
+      <c r="N39" s="3">
+        <v>10.922782</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14">
       <c r="C40" s="3">
         <v>12.810548000000001</v>
       </c>
@@ -1280,20 +1773,35 @@
       <c r="E40" s="2">
         <v>5.8584820000000004</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="3">
         <v>7.0120069999999997</v>
       </c>
       <c r="G40" s="2">
         <v>-2.162623</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <v>28.719988000000001</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="3">
         <v>0.717862</v>
       </c>
-    </row>
-    <row r="41" spans="3:9">
+      <c r="J40" s="2">
+        <v>-1.885734</v>
+      </c>
+      <c r="K40" s="3">
+        <v>5.2931660000000003</v>
+      </c>
+      <c r="L40" s="3">
+        <v>8.7652470000000005</v>
+      </c>
+      <c r="M40" s="3">
+        <v>7.139888</v>
+      </c>
+      <c r="N40" s="3">
+        <v>9.2322469999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14">
       <c r="C41" s="3">
         <v>6.686509</v>
       </c>
@@ -1303,20 +1811,35 @@
       <c r="E41" s="2">
         <v>4.9013179999999998</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="3">
         <v>5.3692719999999996</v>
       </c>
       <c r="G41" s="2">
         <v>0.78422700000000001</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <v>24.393317</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="3">
         <v>0.70357199999999998</v>
       </c>
-    </row>
-    <row r="42" spans="3:9">
+      <c r="J41" s="2">
+        <v>-1.4474130000000001</v>
+      </c>
+      <c r="K41" s="3">
+        <v>4.5814640000000004</v>
+      </c>
+      <c r="L41" s="3">
+        <v>7.5366920000000004</v>
+      </c>
+      <c r="M41" s="3">
+        <v>5.8144679999999997</v>
+      </c>
+      <c r="N41" s="3">
+        <v>7.7409129999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14">
       <c r="C42" s="3">
         <v>6.5144279999999997</v>
       </c>
@@ -1332,14 +1855,29 @@
       <c r="G42" s="2">
         <v>-1.7088479999999999</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>30.103632999999999</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="3">
         <v>0.57577</v>
       </c>
-    </row>
-    <row r="43" spans="3:9">
+      <c r="J42" s="2">
+        <v>-1.2973049999999999</v>
+      </c>
+      <c r="K42" s="3">
+        <v>3.961468</v>
+      </c>
+      <c r="L42" s="3">
+        <v>6.5576020000000002</v>
+      </c>
+      <c r="M42" s="2">
+        <v>4.1381620000000003</v>
+      </c>
+      <c r="N42" s="3">
+        <v>6.5201700000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14">
       <c r="C43" s="2">
         <v>5.8374689999999996</v>
       </c>
@@ -1349,20 +1887,35 @@
       <c r="E43" s="2">
         <v>3.371823</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="3">
         <v>8.1906060000000007</v>
       </c>
       <c r="G43" s="2">
         <v>-1.4412929999999999</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>26.230982999999998</v>
       </c>
       <c r="I43" s="2">
         <v>0.43536799999999998</v>
       </c>
-    </row>
-    <row r="44" spans="3:9">
+      <c r="J43" s="2">
+        <v>-1.107343</v>
+      </c>
+      <c r="K43" s="3">
+        <v>3.3938329999999999</v>
+      </c>
+      <c r="L43" s="3">
+        <v>5.6688179999999999</v>
+      </c>
+      <c r="M43" s="2">
+        <v>3.8042560000000001</v>
+      </c>
+      <c r="N43" s="3">
+        <v>5.6307790000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="3:14">
       <c r="C44" s="2">
         <v>4.7866590000000002</v>
       </c>
@@ -1378,14 +1931,29 @@
       <c r="G44" s="2">
         <v>-1.3170919999999999</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <v>22.782993000000001</v>
       </c>
       <c r="I44" s="2">
         <v>0.42705100000000001</v>
       </c>
-    </row>
-    <row r="45" spans="3:9">
+      <c r="J44" s="2">
+        <v>-0.92805599999999999</v>
+      </c>
+      <c r="K44" s="3">
+        <v>2.8235359999999998</v>
+      </c>
+      <c r="L44" s="3">
+        <v>4.9149849999999997</v>
+      </c>
+      <c r="M44" s="2">
+        <v>3.0484330000000002</v>
+      </c>
+      <c r="N44" s="3">
+        <v>4.5816140000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14">
       <c r="C45" s="2">
         <v>3.7622779999999998</v>
       </c>
@@ -1401,14 +1969,29 @@
       <c r="G45" s="2">
         <v>1.780351</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
         <v>8.0945940000000007</v>
       </c>
       <c r="I45" s="2">
         <v>0.44944000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="3:9">
+      <c r="J45" s="2">
+        <v>-0.85384300000000002</v>
+      </c>
+      <c r="K45" s="3">
+        <v>2.496346</v>
+      </c>
+      <c r="L45" s="3">
+        <v>4.1597289999999996</v>
+      </c>
+      <c r="M45" s="2">
+        <v>2.5588510000000002</v>
+      </c>
+      <c r="N45" s="3">
+        <v>4.0301689999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14">
       <c r="C46" s="2">
         <v>3.2627549999999998</v>
       </c>
@@ -1424,14 +2007,29 @@
       <c r="G46" s="2">
         <v>1.8942399999999999</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="3">
         <v>10.539915000000001</v>
       </c>
       <c r="I46" s="2">
         <v>0.39618799999999998</v>
       </c>
-    </row>
-    <row r="47" spans="3:9">
+      <c r="J46" s="2">
+        <v>-0.71538999999999997</v>
+      </c>
+      <c r="K46" s="3">
+        <v>1.9538070000000001</v>
+      </c>
+      <c r="L46" s="3">
+        <v>3.6346020000000001</v>
+      </c>
+      <c r="M46" s="2">
+        <v>2.0089899999999998</v>
+      </c>
+      <c r="N46" s="3">
+        <v>3.5807169999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14">
       <c r="C47" s="2">
         <v>-2.1091869999999999</v>
       </c>
@@ -1447,14 +2045,29 @@
       <c r="G47" s="2">
         <v>-0.84430700000000003</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
         <v>11.138107</v>
       </c>
       <c r="I47" s="2">
         <v>0.36575600000000003</v>
       </c>
-    </row>
-    <row r="48" spans="3:9">
+      <c r="J47" s="2">
+        <v>-0.51270300000000002</v>
+      </c>
+      <c r="K47" s="3">
+        <v>1.863027</v>
+      </c>
+      <c r="L47" s="3">
+        <v>3.116098</v>
+      </c>
+      <c r="M47" s="2">
+        <v>1.5801750000000001</v>
+      </c>
+      <c r="N47" s="2">
+        <v>3.117245</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14">
       <c r="C48" s="2">
         <v>2.419556</v>
       </c>
@@ -1470,14 +2083,29 @@
       <c r="G48" s="2">
         <v>-0.69787200000000005</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="3">
         <v>13.476260999999999</v>
       </c>
       <c r="I48" s="2">
         <v>0.38389299999999998</v>
       </c>
-    </row>
-    <row r="49" spans="3:9">
+      <c r="J48" s="2">
+        <v>-0.421844</v>
+      </c>
+      <c r="K48" s="3">
+        <v>1.58961</v>
+      </c>
+      <c r="L48" s="3">
+        <v>2.7463920000000002</v>
+      </c>
+      <c r="M48" s="2">
+        <v>0.89776500000000004</v>
+      </c>
+      <c r="N48" s="2">
+        <v>2.4693939999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14">
       <c r="C49" s="2">
         <v>2.3465579999999999</v>
       </c>
@@ -1487,20 +2115,35 @@
       <c r="E49" s="2">
         <v>1.3877299999999999</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="3">
         <v>6.5509909999999998</v>
       </c>
       <c r="G49" s="2">
         <v>-0.64917599999999998</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="3">
         <v>12.237821</v>
       </c>
       <c r="I49" s="2">
         <v>0.272565</v>
       </c>
-    </row>
-    <row r="50" spans="3:9">
+      <c r="J49" s="2">
+        <v>-0.30507899999999999</v>
+      </c>
+      <c r="K49" s="3">
+        <v>1.3136760000000001</v>
+      </c>
+      <c r="L49" s="3">
+        <v>2.5646960000000001</v>
+      </c>
+      <c r="M49" s="2">
+        <v>0.82345100000000004</v>
+      </c>
+      <c r="N49" s="2">
+        <v>2.2256879999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14">
       <c r="C50" s="2">
         <v>8.2633930000000007</v>
       </c>
@@ -1516,14 +2159,29 @@
       <c r="G50" s="2">
         <v>-0.53462100000000001</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
         <v>6.4197119999999996</v>
       </c>
       <c r="I50" s="2">
         <v>0.19303899999999999</v>
       </c>
-    </row>
-    <row r="51" spans="3:9">
+      <c r="J50" s="2">
+        <v>-0.28939300000000001</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1.1839900000000001</v>
+      </c>
+      <c r="L50" s="3">
+        <v>2.1492969999999998</v>
+      </c>
+      <c r="M50" s="2">
+        <v>0.62663899999999995</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1.8046340000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14">
       <c r="C51" s="2">
         <v>1.5927770000000001</v>
       </c>
@@ -1545,8 +2203,23 @@
       <c r="I51" s="2">
         <v>0.12643199999999999</v>
       </c>
-    </row>
-    <row r="52" spans="3:9">
+      <c r="J51" s="2">
+        <v>-0.34154400000000001</v>
+      </c>
+      <c r="K51" s="3">
+        <v>1.0447960000000001</v>
+      </c>
+      <c r="L51" s="3">
+        <v>1.995231</v>
+      </c>
+      <c r="M51" s="2">
+        <v>0.36761100000000002</v>
+      </c>
+      <c r="N51" s="2">
+        <v>1.695778</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14">
       <c r="C52" s="2">
         <v>3.1834289999999998</v>
       </c>
@@ -1562,14 +2235,29 @@
       <c r="G52" s="2">
         <v>-0.16978299999999999</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="3">
         <v>4.3689280000000004</v>
       </c>
       <c r="I52" s="2">
         <v>0.120918</v>
       </c>
-    </row>
-    <row r="53" spans="3:9">
+      <c r="J52" s="2">
+        <v>-0.32077099999999997</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.83736900000000003</v>
+      </c>
+      <c r="L52" s="3">
+        <v>1.689597</v>
+      </c>
+      <c r="M52" s="2">
+        <v>0.19831299999999999</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1.6160270000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14">
       <c r="C53" s="2">
         <v>1.309442</v>
       </c>
@@ -1585,14 +2273,29 @@
       <c r="G53" s="2">
         <v>-0.28432299999999999</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="3">
         <v>8.1003910000000001</v>
       </c>
       <c r="I53" s="2">
         <v>0.122061</v>
       </c>
-    </row>
-    <row r="54" spans="3:9">
+      <c r="J53" s="2">
+        <v>-0.188805</v>
+      </c>
+      <c r="K53" s="3">
+        <v>0.68956499999999998</v>
+      </c>
+      <c r="L53" s="3">
+        <v>1.4990209999999999</v>
+      </c>
+      <c r="M53" s="2">
+        <v>-2.0604999999999998E-2</v>
+      </c>
+      <c r="N53" s="2">
+        <v>-1.1046180000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14">
       <c r="C54" s="2">
         <v>1.2655829999999999</v>
       </c>
@@ -1608,14 +2311,29 @@
       <c r="G54" s="2">
         <v>-0.31613000000000002</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="3">
         <v>7.1374069999999996</v>
       </c>
       <c r="I54" s="2">
         <v>0.101939</v>
       </c>
-    </row>
-    <row r="55" spans="3:9">
+      <c r="J54" s="2">
+        <v>-0.25172800000000001</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.63922199999999996</v>
+      </c>
+      <c r="L54" s="3">
+        <v>1.289207</v>
+      </c>
+      <c r="M54" s="2">
+        <v>-0.152472</v>
+      </c>
+      <c r="N54" s="2">
+        <v>-1.2532509999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="3:14">
       <c r="C55" s="2">
         <v>1.135229</v>
       </c>
@@ -1631,14 +2349,29 @@
       <c r="G55" s="2">
         <v>-0.25728699999999999</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="3">
         <v>6.9921569999999997</v>
       </c>
       <c r="I55" s="2">
         <v>0.18090000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="3:9">
+      <c r="J55" s="2">
+        <v>-0.30599300000000001</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.62032200000000004</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1.2286760000000001</v>
+      </c>
+      <c r="M55" s="2">
+        <v>-0.25679200000000002</v>
+      </c>
+      <c r="N55" s="2">
+        <v>-0.48084199999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14">
       <c r="C56" s="2">
         <v>0.93454999999999999</v>
       </c>
@@ -1654,14 +2387,29 @@
       <c r="G56" s="2">
         <v>-0.21987599999999999</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="3">
         <v>6.6224129999999999</v>
       </c>
       <c r="I56" s="2">
         <v>0.109376</v>
       </c>
-    </row>
-    <row r="57" spans="3:9">
+      <c r="J56" s="2">
+        <v>-0.27367399999999997</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0.542188</v>
+      </c>
+      <c r="L56" s="3">
+        <v>1.1033230000000001</v>
+      </c>
+      <c r="M56" s="2">
+        <v>-0.197246</v>
+      </c>
+      <c r="N56" s="2">
+        <v>-1.792408</v>
+      </c>
+    </row>
+    <row r="57" spans="3:14">
       <c r="C57" s="2">
         <v>0.81896400000000003</v>
       </c>
@@ -1677,14 +2425,29 @@
       <c r="G57" s="2">
         <v>-0.21063699999999999</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="3">
         <v>6.021102</v>
       </c>
       <c r="I57" s="2">
         <v>0.18452499999999999</v>
       </c>
-    </row>
-    <row r="58" spans="3:9">
+      <c r="J57" s="2">
+        <v>-0.16763800000000001</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0.44233899999999998</v>
+      </c>
+      <c r="L57" s="3">
+        <v>1.0423709999999999</v>
+      </c>
+      <c r="M57" s="2">
+        <v>-0.27302199999999999</v>
+      </c>
+      <c r="N57" s="2">
+        <v>-1.3017259999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14">
       <c r="C58" s="2">
         <v>0.73578100000000002</v>
       </c>
@@ -1700,11 +2463,26 @@
       <c r="G58" s="2">
         <v>-9.8483000000000001E-2</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="3">
         <v>5.6475080000000002</v>
       </c>
       <c r="I58" s="2">
         <v>0.11527800000000001</v>
+      </c>
+      <c r="J58" s="2">
+        <v>-0.11643000000000001</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0.43738199999999999</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0.706148</v>
+      </c>
+      <c r="M58" s="2">
+        <v>-0.29575699999999999</v>
+      </c>
+      <c r="N58" s="2">
+        <v>-1.924156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plotted all the new graphs on one single scale
</commit_message>
<xml_diff>
--- a/Initial_Data_Analysis.xlsx
+++ b/Initial_Data_Analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Leaf 1</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>For File1</t>
+  </si>
+  <si>
+    <t>Probabilities</t>
+  </si>
+  <si>
+    <t>no failure</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -122,6 +128,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,21 +423,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N58"/>
+  <dimension ref="B2:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:28">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:28">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -467,8 +476,47 @@
       <c r="N3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -509,7 +557,63 @@
         <v>3.262858</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="5" spans="2:28">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" ref="R5:AB21" si="0">1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28">
       <c r="C7" s="2">
         <v>0.179512</v>
       </c>
@@ -546,8 +650,59 @@
       <c r="N7" s="2">
         <v>0.23070599999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
+      <c r="P7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q7" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB7" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28">
       <c r="C8" s="2">
         <v>0.19955999999999999</v>
       </c>
@@ -584,8 +739,59 @@
       <c r="N8" s="2">
         <v>0.14523</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="P8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28">
       <c r="C9" s="2">
         <v>0.190305</v>
       </c>
@@ -622,8 +828,59 @@
       <c r="N9" s="2">
         <v>0.19728000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
+      <c r="P9" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28">
       <c r="C10" s="2">
         <v>0.21299599999999999</v>
       </c>
@@ -660,8 +917,59 @@
       <c r="N10" s="2">
         <v>0.10732700000000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="P10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28">
       <c r="C11" s="2">
         <v>0.25013600000000002</v>
       </c>
@@ -698,8 +1006,59 @@
       <c r="N11" s="2">
         <v>8.1478999999999996E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="P11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q11" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28">
       <c r="C12" s="2">
         <v>0.25830799999999998</v>
       </c>
@@ -736,8 +1095,59 @@
       <c r="N12" s="2">
         <v>0.263241</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
+      <c r="P12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB12" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28">
       <c r="C13" s="2">
         <v>0.267152</v>
       </c>
@@ -774,8 +1184,59 @@
       <c r="N13" s="2">
         <v>0.19262099999999999</v>
       </c>
-    </row>
-    <row r="14" spans="2:14">
+      <c r="P13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB13" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28">
       <c r="C14" s="2">
         <v>0.25653599999999999</v>
       </c>
@@ -812,8 +1273,59 @@
       <c r="N14" s="2">
         <v>5.3763999999999999E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:14">
+      <c r="P14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q14" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB14" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28">
       <c r="C15" s="2">
         <v>4.9303410000000003</v>
       </c>
@@ -850,8 +1362,59 @@
       <c r="N15" s="2">
         <v>0.233594</v>
       </c>
-    </row>
-    <row r="16" spans="2:14">
+      <c r="P15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q15" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB15" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28">
       <c r="C16" s="2">
         <v>5.4243740000000003</v>
       </c>
@@ -888,8 +1451,59 @@
       <c r="N16" s="2">
         <v>0.39887099999999998</v>
       </c>
-    </row>
-    <row r="17" spans="3:14">
+      <c r="P16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q16" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:28">
       <c r="C17" s="2">
         <v>5.0024629999999997</v>
       </c>
@@ -926,8 +1540,59 @@
       <c r="N17" s="2">
         <v>0.373417</v>
       </c>
-    </row>
-    <row r="18" spans="3:14">
+      <c r="P17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB17" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:28">
       <c r="C18" s="2">
         <v>3.2428379999999999</v>
       </c>
@@ -964,8 +1629,59 @@
       <c r="N18" s="2">
         <v>0.30244399999999999</v>
       </c>
-    </row>
-    <row r="19" spans="3:14">
+      <c r="P18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB18" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:28">
       <c r="C19" s="2">
         <v>0.28927599999999998</v>
       </c>
@@ -1002,8 +1718,59 @@
       <c r="N19" s="2">
         <v>0.41719800000000001</v>
       </c>
-    </row>
-    <row r="20" spans="3:14">
+      <c r="P19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB19" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:28">
       <c r="C20" s="2">
         <v>0.25277300000000003</v>
       </c>
@@ -1040,8 +1807,59 @@
       <c r="N20" s="2">
         <v>0.68149000000000004</v>
       </c>
-    </row>
-    <row r="21" spans="3:14">
+      <c r="P20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q20" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:28">
       <c r="C21" s="2">
         <v>0.21038699999999999</v>
       </c>
@@ -1078,8 +1896,59 @@
       <c r="N21" s="2">
         <v>0.57286599999999999</v>
       </c>
-    </row>
-    <row r="22" spans="3:14">
+      <c r="P21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q21" s="4">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="Z21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AA21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="AB21" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:28">
       <c r="C22" s="2">
         <v>5.2755580000000002</v>
       </c>
@@ -1117,7 +1986,7 @@
         <v>2.0498980000000002</v>
       </c>
     </row>
-    <row r="23" spans="3:14">
+    <row r="23" spans="3:28">
       <c r="C23" s="3">
         <v>8.5485489999999995</v>
       </c>
@@ -1155,7 +2024,7 @@
         <v>6.095529</v>
       </c>
     </row>
-    <row r="24" spans="3:14">
+    <row r="24" spans="3:28">
       <c r="C24" s="2">
         <v>-8.6788830000000008</v>
       </c>
@@ -1193,7 +2062,7 @@
         <v>10.548679999999999</v>
       </c>
     </row>
-    <row r="25" spans="3:14">
+    <row r="25" spans="3:28">
       <c r="C25" s="3">
         <v>10.932235</v>
       </c>
@@ -1231,7 +2100,7 @@
         <v>11.304500000000001</v>
       </c>
     </row>
-    <row r="26" spans="3:14">
+    <row r="26" spans="3:28">
       <c r="C26" s="3">
         <v>13.904157</v>
       </c>
@@ -1269,7 +2138,7 @@
         <v>13.433028</v>
       </c>
     </row>
-    <row r="27" spans="3:14">
+    <row r="27" spans="3:28">
       <c r="C27" s="2">
         <v>5.3677400000000004</v>
       </c>
@@ -1307,7 +2176,7 @@
         <v>15.265772999999999</v>
       </c>
     </row>
-    <row r="28" spans="3:14">
+    <row r="28" spans="3:28">
       <c r="C28" s="3">
         <v>19.491105999999998</v>
       </c>
@@ -1345,7 +2214,7 @@
         <v>16.958817</v>
       </c>
     </row>
-    <row r="29" spans="3:14">
+    <row r="29" spans="3:28">
       <c r="C29" s="3">
         <v>16.106985000000002</v>
       </c>
@@ -1383,7 +2252,7 @@
         <v>18.528184</v>
       </c>
     </row>
-    <row r="30" spans="3:14">
+    <row r="30" spans="3:28">
       <c r="C30" s="3">
         <v>17.095763000000002</v>
       </c>
@@ -1421,7 +2290,7 @@
         <v>20.592317999999999</v>
       </c>
     </row>
-    <row r="31" spans="3:14">
+    <row r="31" spans="3:28">
       <c r="C31" s="3">
         <v>17.972626000000002</v>
       </c>
@@ -1459,7 +2328,7 @@
         <v>20.790599</v>
       </c>
     </row>
-    <row r="32" spans="3:14">
+    <row r="32" spans="3:28">
       <c r="C32" s="3">
         <v>18.692540999999999</v>
       </c>

</xml_diff>

<commit_message>
changed code to remove all NaN entries and recalculated % changes
</commit_message>
<xml_diff>
--- a/Initial_Data_Analysis.xlsx
+++ b/Initial_Data_Analysis.xlsx
@@ -425,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AB58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
@@ -654,7 +654,7 @@
         <v>0.5</v>
       </c>
       <c r="Q7" s="4">
-        <f>1/24</f>
+        <f t="shared" ref="Q7:Q21" si="1">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R7" s="4">
@@ -743,7 +743,7 @@
         <v>0.5</v>
       </c>
       <c r="Q8" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R8" s="4">
@@ -832,7 +832,7 @@
         <v>0.5</v>
       </c>
       <c r="Q9" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R9" s="4">
@@ -921,7 +921,7 @@
         <v>0.5</v>
       </c>
       <c r="Q10" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R10" s="4">
@@ -1010,7 +1010,7 @@
         <v>0.5</v>
       </c>
       <c r="Q11" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R11" s="4">
@@ -1099,7 +1099,7 @@
         <v>0.5</v>
       </c>
       <c r="Q12" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R12" s="4">
@@ -1188,7 +1188,7 @@
         <v>0.5</v>
       </c>
       <c r="Q13" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R13" s="4">
@@ -1277,7 +1277,7 @@
         <v>0.5</v>
       </c>
       <c r="Q14" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R14" s="4">
@@ -1366,7 +1366,7 @@
         <v>0.5</v>
       </c>
       <c r="Q15" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R15" s="4">
@@ -1455,7 +1455,7 @@
         <v>0.5</v>
       </c>
       <c r="Q16" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R16" s="4">
@@ -1544,7 +1544,7 @@
         <v>0.5</v>
       </c>
       <c r="Q17" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R17" s="4">
@@ -1633,7 +1633,7 @@
         <v>0.5</v>
       </c>
       <c r="Q18" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R18" s="4">
@@ -1722,7 +1722,7 @@
         <v>0.5</v>
       </c>
       <c r="Q19" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R19" s="4">
@@ -1811,7 +1811,7 @@
         <v>0.5</v>
       </c>
       <c r="Q20" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R20" s="4">
@@ -1900,7 +1900,7 @@
         <v>0.5</v>
       </c>
       <c r="Q21" s="4">
-        <f>1/24</f>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R21" s="4">

</xml_diff>